<commit_message>
Add much more detail to command interpreter, add tests
</commit_message>
<xml_diff>
--- a/tests/ht_matrix.xlsx
+++ b/tests/ht_matrix.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <s:workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <s:bookViews>
-    <s:workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
-  </s:bookViews>
-  <s:sheets>
-    <s:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="rId1"/>
-  </s:sheets>
-  <s:definedNames/>
-  <s:calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
-</s:workbook>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26423"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <bookViews>
+    <workbookView xWindow="7160" yWindow="8160" windowWidth="25600" windowHeight="15620"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+  </sheets>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Peak Period</t>
-  </si>
-  <si>
-    <t>Percent</t>
   </si>
   <si>
     <t>Significant Wave Height</t>
@@ -29,9 +30,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -58,16 +58,16 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -392,201 +392,153 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryRight="1" summaryBelow="1"/>
-  </sheetPr>
-  <dimension ref="A1:C16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col width="22.83203125" min="1" customWidth="1" max="1"/>
-    <col width="9.10" min="2" max="2"/>
-    <col width="9.10" min="3" max="3"/>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row spans="1:3" r="1">
-      <c t="s" r="A1">
-        <v>2</v>
-      </c>
-      <c t="s" r="B1">
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c t="s" r="C1">
-        <v>1</v>
-      </c>
-    </row>
-    <row spans="1:3" r="2">
-      <c t="n" r="A2">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
         <v>1.75</v>
       </c>
-      <c t="n" r="B2">
+      <c r="B2">
         <v>5.8</v>
       </c>
-      <c t="n" r="C2">
-        <v>1.0649999999999995</v>
-      </c>
-    </row>
-    <row spans="1:3" r="3">
-      <c t="n" r="A3">
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
         <v>3.5</v>
       </c>
-      <c t="n" r="B3">
-        <v>8.2</v>
-      </c>
-      <c t="n" r="C3">
-        <v>0.9254999999999993</v>
-      </c>
-    </row>
-    <row spans="1:3" r="4">
-      <c t="n" r="A4">
+      <c r="B3">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
         <v>5.9</v>
       </c>
-      <c t="n" r="B4">
+      <c r="B4">
         <v>10.65</v>
       </c>
-      <c t="n" r="C4">
-        <v>0.002100000000000003</v>
-      </c>
-    </row>
-    <row spans="1:3" r="5">
-      <c t="n" r="A5">
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
         <v>2.5</v>
       </c>
-      <c t="n" r="B5">
-        <v>8.95</v>
-      </c>
-      <c t="n" r="C5">
-        <v>3.5359999999999996</v>
-      </c>
-    </row>
-    <row spans="1:3" r="6">
-      <c t="n" r="A6">
+      <c r="B5">
+        <v>8.9499999999999993</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
         <v>4.45</v>
       </c>
-      <c t="n" r="B6">
+      <c r="B6">
         <v>11.95</v>
       </c>
-      <c t="n" r="C6">
-        <v>0.4849999999999998</v>
-      </c>
-    </row>
-    <row spans="1:3" r="7">
-      <c t="n" r="A7">
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
         <v>6.5</v>
       </c>
-      <c t="n" r="B7">
+      <c r="B7">
         <v>15</v>
       </c>
-      <c t="n" r="C7">
-        <v>0.0125</v>
-      </c>
-    </row>
-    <row spans="1:3" r="8">
-      <c t="n" r="A8">
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
         <v>1.25</v>
       </c>
-      <c t="n" r="B8">
+      <c r="B8">
         <v>7.5</v>
       </c>
-      <c t="n" r="C8">
-        <v>5.56</v>
-      </c>
-    </row>
-    <row spans="1:3" r="9">
-      <c t="n" r="A9">
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
         <v>3.5</v>
       </c>
-      <c t="n" r="B9">
+      <c r="B9">
         <v>12.55</v>
       </c>
-      <c t="n" r="C9">
-        <v>0.6937499999999999</v>
-      </c>
-    </row>
-    <row spans="1:3" r="10">
-      <c t="n" r="A10">
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
         <v>5.2</v>
       </c>
-      <c t="n" r="B10">
+      <c r="B10">
         <v>15.5</v>
       </c>
-      <c t="n" r="C10">
-        <v>0.020000000000000004</v>
-      </c>
-    </row>
-    <row spans="1:3" r="11">
-      <c t="n" r="A11">
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
         <v>1.75</v>
       </c>
-      <c t="n" r="B11">
-        <v>10.05</v>
-      </c>
-      <c t="n" r="C11">
-        <v>2.9289999999999985</v>
-      </c>
-    </row>
-    <row spans="1:3" r="12">
-      <c t="n" r="A12">
+      <c r="B11">
+        <v>10.050000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
         <v>2.7</v>
       </c>
-      <c t="n" r="B12">
+      <c r="B12">
         <v>12.5</v>
       </c>
-      <c t="n" r="C12">
-        <v>0.7780000000000001</v>
-      </c>
-    </row>
-    <row spans="1:3" r="13">
-      <c t="n" r="A13">
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
         <v>3.7</v>
       </c>
-      <c t="n" r="B13">
+      <c r="B13">
         <v>14.75</v>
       </c>
-      <c t="n" r="C13">
-        <v>0.08825000000000001</v>
-      </c>
-    </row>
-    <row spans="1:3" r="14">
-      <c t="n" r="A14">
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
         <v>1.35</v>
       </c>
-      <c t="n" r="B14">
+      <c r="B14">
         <v>11.4</v>
       </c>
-      <c t="n" r="C14">
-        <v>0.25259999999999977</v>
-      </c>
-    </row>
-    <row spans="1:3" r="15">
-      <c t="n" r="A15">
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
         <v>2.65</v>
       </c>
-      <c t="n" r="B15">
+      <c r="B15">
         <v>16.3</v>
       </c>
-      <c t="n" r="C15">
-        <v>0.03199999999999998</v>
-      </c>
-    </row>
-    <row spans="1:3" r="16">
-      <c t="n" r="A16">
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
         <v>3.8</v>
       </c>
-      <c t="n" r="B16">
+      <c r="B16">
         <v>20.45</v>
       </c>
-      <c t="n" r="C16">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1.00" bottom="1.00" header="0.50" footer="0.50"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>